<commit_message>
Final document grading requirements
</commit_message>
<xml_diff>
--- a/Documents/Grading Requirements.xlsx
+++ b/Documents/Grading Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.liu.se\home\chrvo878\Documents\TDDC88\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45BB1CD5-A61C-4FB6-A870-F9C3AFD2B1BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BB2A42-8551-495F-93E9-2F37647FABEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{A4E57E99-9CA4-4DEC-8ED6-1C87B0EAD57F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Technical grading requirements</t>
   </si>
@@ -77,12 +77,15 @@
   <si>
     <t>Value</t>
   </si>
+  <si>
+    <t>Weekly status report</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,11 +99,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -141,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -150,38 +148,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -189,86 +156,32 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -393,7 +306,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2BFE9E9-2783-4098-8448-EE22EDEADCAC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -460,7 +373,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22D524CF-0A90-4B36-8708-D26A232FCC21}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -527,7 +440,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2618853F-2336-401A-AC69-D09248913DDA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -594,7 +507,7 @@
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49E5A66A-9E14-42C7-83B1-820F3D898500}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -661,7 +574,7 @@
                   <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DDB5C0F-8C71-4180-B472-F8720B56DB46}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -728,7 +641,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37BE940C-2BCB-4533-AFE3-B718A4A7E13D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -795,7 +708,7 @@
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E0B7621-BF1A-4B28-9CD0-0FE8A484593B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -862,7 +775,7 @@
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E860C5F3-7867-403D-A616-CB0984702ED8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -929,7 +842,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D51B320C-A71E-4140-A912-74A1CEA461A7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -996,7 +909,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954BD057-67F0-4B01-A10A-E712E839CA28}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1052,8 +965,8 @@
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>114300</xdr:colOff>
-          <xdr:row>14</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1063,7 +976,7 @@
                   <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E4313E3-DE13-4A2B-BC64-EF7869F8A66E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1407,10 +1320,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34383DD3-494A-4DB4-8286-B8F7C91FF2B1}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,138 +1331,156 @@
     <col min="1" max="1" width="113.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="D1" s="9" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="6" t="b">
         <v>0</v>
       </c>
+      <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6" t="b">
+      <c r="B4" s="6"/>
+      <c r="C4" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="b">
+      <c r="B5" s="6"/>
+      <c r="C5" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="6" t="b">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="6" t="b">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="6" t="b">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="D9" s="11"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="6" t="b">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="6" t="b">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="D12" s="11"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="6" t="b">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="D13" s="11"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="6" t="b">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="D14" s="11"/>
     </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11" t="b">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="D15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1558,10 +1489,10 @@
     <mergeCell ref="B11:C11"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:C2">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>COUNTIF($C3:$C5, FALSE)=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>COUNTIF($C3:$C5, FALSE) &lt;&gt; 0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1822,8 +1753,8 @@
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>114300</xdr:colOff>
-                    <xdr:row>14</xdr:row>
-                    <xdr:rowOff>190500</xdr:rowOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>